<commit_message>
Frontend scaffolding for general sections (e.g. items, vendors, etc.).
</commit_message>
<xml_diff>
--- a/WorkBot/main/backend/ordering/OrderFiles/Regional Distributors, Inc/Regional Distributors, Inc._Bakery_20250629.xlsx
+++ b/WorkBot/main/backend/ordering/OrderFiles/Regional Distributors, Inc/Regional Distributors, Inc._Bakery_20250629.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E20"/>
+  <dimension ref="A1:E22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -961,6 +961,60 @@
         </is>
       </c>
     </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>38505</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>Container - Paper Clamshell (Avocado Box)</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t>56.85</t>
+        </is>
+      </c>
+      <c r="E21" t="inlineStr">
+        <is>
+          <t>56.85</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>22517</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>Bag Sheet Pan Cover 30x43</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="D22" t="inlineStr">
+        <is>
+          <t>27.77</t>
+        </is>
+      </c>
+      <c r="E22" t="inlineStr">
+        <is>
+          <t>55.54</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>